<commit_message>
wrangled the new datasets and merged them into one for the linear models. developed three models. Currently working on write-up describing them.
</commit_message>
<xml_diff>
--- a/Data/Raw/US CDC - Death Rate 2021.xlsx
+++ b/Data/Raw/US CDC - Death Rate 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Homework\ENV 872 Environmental Data Analytics\EDA_Class_Project_Sp23\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F072ABE-5545-4CB5-BDFB-834B7D9675B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5790A0B0-BEBD-4E9E-A4CC-3C0C7E30340B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8CF41DB4-13D1-4BCE-82FB-AB98A4AF99F3}"/>
   </bookViews>
@@ -234,6 +234,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -271,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -279,13 +282,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -605,23 +605,27 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -647,19 +651,19 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>58054</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>59.5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>68889</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>1366.9</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>1134.2</v>
       </c>
     </row>
@@ -667,19 +671,19 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>9367</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>64.900000000000006</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>6208</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>847.3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>931</v>
       </c>
     </row>
@@ -687,19 +691,19 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>77916</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>55.5</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>81442</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>1119.3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>908.5</v>
       </c>
     </row>
@@ -707,39 +711,39 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>35965</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>61.7</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>40070</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>1324.2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>1097.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>420608</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>52.8</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>333249</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>849.3</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>760.4</v>
       </c>
     </row>
@@ -747,39 +751,39 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>62949</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>52.5</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>48281</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>830.7</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>799</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>35670</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>52.1</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>34333</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>952.2</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <v>725.1</v>
       </c>
     </row>
@@ -787,39 +791,39 @@
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>10482</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>56.5</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>11296</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>1125.8</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <v>867</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>8660</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>48.7</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="4">
         <v>5833</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>870.5</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>868.5</v>
       </c>
     </row>
@@ -827,19 +831,19 @@
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>216260</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>54.9</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="4">
         <v>261369</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>1200</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>832.9</v>
       </c>
     </row>
@@ -847,19 +851,19 @@
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>124073</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>55.9</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="4">
         <v>112272</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>1039.5999999999999</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="3">
         <v>997.6</v>
       </c>
     </row>
@@ -867,19 +871,19 @@
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>15620</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>59.2</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <v>12816</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>889</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="3">
         <v>630</v>
       </c>
     </row>
@@ -887,19 +891,19 @@
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="4">
         <v>22427</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>60.7</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="4">
         <v>18346</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>965.1</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <v>881</v>
       </c>
     </row>
@@ -907,19 +911,19 @@
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <v>132189</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>53</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <v>125048</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>986.8</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="3">
         <v>825.3</v>
       </c>
     </row>
@@ -927,19 +931,19 @@
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>79946</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>60.2</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="4">
         <v>78317</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>1150.7</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="3">
         <v>999.3</v>
       </c>
     </row>
@@ -947,19 +951,19 @@
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="4">
         <v>36835</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>60.8</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="4">
         <v>34215</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>1071.5</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="3">
         <v>841.8</v>
       </c>
     </row>
@@ -967,19 +971,19 @@
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="4">
         <v>34705</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>61</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="4">
         <v>32029</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>1091.4000000000001</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
         <v>915</v>
       </c>
     </row>
@@ -987,19 +991,19 @@
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <v>52214</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>60.8</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="4">
         <v>60303</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>1337.3</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>1139.5999999999999</v>
       </c>
     </row>
@@ -1007,19 +1011,19 @@
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>57437</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>62.7</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="4">
         <v>57533</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>1244.2</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>1094.5999999999999</v>
       </c>
     </row>
@@ -1027,59 +1031,59 @@
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>12006</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>49.9</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="4">
         <v>17269</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>1258.4000000000001</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="3">
         <v>889.4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>68285</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <v>56.4</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="4">
         <v>58117</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="3">
         <v>942.7</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="3">
         <v>805.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="4">
         <v>69137</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="3">
         <v>49</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="4">
         <v>63115</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="3">
         <v>903.6</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="3">
         <v>721.4</v>
       </c>
     </row>
@@ -1087,19 +1091,19 @@
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="4">
         <v>104980</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <v>55.4</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="4">
         <v>117782</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>1171.9000000000001</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="3">
         <v>943.1</v>
       </c>
     </row>
@@ -1107,19 +1111,19 @@
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>64425</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="3">
         <v>58.6</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="4">
         <v>51640</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="3">
         <v>904.8</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="3">
         <v>756.5</v>
       </c>
     </row>
@@ -1127,19 +1131,19 @@
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="4">
         <v>35156</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <v>60.7</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="4">
         <v>41085</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>1392.7</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <v>1204.5</v>
       </c>
     </row>
@@ -1147,19 +1151,19 @@
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>69453</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="3">
         <v>58.4</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="4">
         <v>73847</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>1197.2</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="3">
         <v>971.9</v>
       </c>
     </row>
@@ -1167,19 +1171,19 @@
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="4">
         <v>11231</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <v>54.8</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="4">
         <v>12707</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>1150.7</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="3">
         <v>909.9</v>
       </c>
     </row>
@@ -1187,19 +1191,19 @@
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="4">
         <v>24609</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="3">
         <v>64.400000000000006</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="4">
         <v>18925</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="3">
         <v>963.7</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="3">
         <v>818.6</v>
       </c>
     </row>
@@ -1207,19 +1211,19 @@
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>33686</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="3">
         <v>54.8</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="4">
         <v>32923</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>1047.2</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="3">
         <v>937.3</v>
       </c>
     </row>
@@ -1227,19 +1231,19 @@
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="4">
         <v>12625</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="3">
         <v>49.9</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="4">
         <v>14198</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>1022.2</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="3">
         <v>782.9</v>
       </c>
     </row>
@@ -1247,19 +1251,19 @@
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="4">
         <v>101497</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="3">
         <v>58</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="4">
         <v>84032</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="3">
         <v>906.8</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="3">
         <v>731.1</v>
       </c>
     </row>
@@ -1267,19 +1271,19 @@
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="4">
         <v>21391</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="3">
         <v>52.9</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="4">
         <v>25300</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>1195.7</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="3">
         <v>995.5</v>
       </c>
     </row>
@@ -1287,19 +1291,19 @@
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="4">
         <v>210742</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="3">
         <v>54.1</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="4">
         <v>181360</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="3">
         <v>914.3</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="3">
         <v>713.1</v>
       </c>
     </row>
@@ -1307,19 +1311,19 @@
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="4">
         <v>120466</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="3">
         <v>58.1</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="4">
         <v>118093</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>1119.2</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="3">
         <v>960</v>
       </c>
     </row>
@@ -1327,19 +1331,19 @@
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="4">
         <v>10112</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="3">
         <v>66.7</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="4">
         <v>7266</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="3">
         <v>937.6</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="3">
         <v>794.2</v>
       </c>
     </row>
@@ -1347,19 +1351,19 @@
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="4">
         <v>129791</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="3">
         <v>57.9</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="4">
         <v>147635</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>1253.3</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="3">
         <v>1012.8</v>
       </c>
     </row>
@@ -1367,19 +1371,19 @@
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="4">
         <v>48410</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="3">
         <v>61.5</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="4">
         <v>50945</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>1277.9000000000001</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="3">
         <v>1121.0999999999999</v>
       </c>
     </row>
@@ -1387,19 +1391,19 @@
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="4">
         <v>40914</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="3">
         <v>48.9</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="4">
         <v>44989</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>1059.5</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="3">
         <v>861</v>
       </c>
     </row>
@@ -1407,19 +1411,19 @@
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="4">
         <v>132622</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="3">
         <v>54.7</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="4">
         <v>155390</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>1198.5999999999999</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="3">
         <v>895</v>
       </c>
     </row>
@@ -1427,19 +1431,19 @@
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="4">
         <v>10464</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="3">
         <v>48.3</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="4">
         <v>11243</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <v>1026.2</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="3">
         <v>781.3</v>
       </c>
     </row>
@@ -1447,19 +1451,19 @@
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="4">
         <v>57185</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="3">
         <v>57.5</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="4">
         <v>65422</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="3">
         <v>1260.4000000000001</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="3">
         <v>1038.0999999999999</v>
       </c>
     </row>
@@ -1467,19 +1471,19 @@
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="4">
         <v>11369</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="3">
         <v>68.599999999999994</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="4">
         <v>9185</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="3">
         <v>1025.8</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="3">
         <v>858.9</v>
       </c>
     </row>
@@ -1487,19 +1491,19 @@
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="4">
         <v>81717</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="3">
         <v>59.8</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="4">
         <v>91130</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="3">
         <v>1306.5</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="3">
         <v>1121.3</v>
       </c>
     </row>
@@ -1507,19 +1511,19 @@
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="4">
         <v>373594</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="3">
         <v>60.7</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="4">
         <v>267651</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="3">
         <v>906.4</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="3">
         <v>942.1</v>
       </c>
     </row>
@@ -1527,19 +1531,19 @@
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="4">
         <v>46712</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="3">
         <v>63.6</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="4">
         <v>22569</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="3">
         <v>676.1</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="3">
         <v>815.8</v>
       </c>
     </row>
@@ -1547,19 +1551,19 @@
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="4">
         <v>5384</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="3">
         <v>44.9</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="4">
         <v>6877</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="3">
         <v>1065.3</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="3">
         <v>791.2</v>
       </c>
     </row>
@@ -1567,19 +1571,19 @@
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="4">
         <v>95825</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="3">
         <v>56.1</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="4">
         <v>85940</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="3">
         <v>994.4</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="3">
         <v>866.5</v>
       </c>
     </row>
@@ -1587,19 +1591,19 @@
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="4">
         <v>83911</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="3">
         <v>54.2</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="4">
         <v>68689</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="3">
         <v>887.6</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="3">
         <v>796.4</v>
       </c>
     </row>
@@ -1607,19 +1611,19 @@
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="4">
         <v>17198</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="3">
         <v>54.7</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="4">
         <v>29503</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="3">
         <v>1654.7</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51" s="3">
         <v>1229.0999999999999</v>
       </c>
     </row>
@@ -1627,19 +1631,19 @@
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="4">
         <v>61781</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="3">
         <v>55.7</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="4">
         <v>60973</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="3">
         <v>1034.2</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F52" s="3">
         <v>837</v>
       </c>
     </row>
@@ -1647,19 +1651,19 @@
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="4">
         <v>6237</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="3">
         <v>57.5</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="4">
         <v>6582</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="3">
         <v>1137.2</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="3">
         <v>954.7</v>
       </c>
     </row>
@@ -1667,19 +1671,19 @@
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="4">
         <v>19304</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="3">
         <v>30.8</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="4">
         <v>33001</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="3">
         <v>1011.2</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="3">
         <v>634.70000000000005</v>
       </c>
     </row>
@@ -1687,19 +1691,19 @@
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="4">
         <v>903</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="3">
         <v>48.4</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="4">
         <v>747</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="3">
         <v>705.6</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="3">
         <v>568.79999999999995</v>
       </c>
     </row>
@@ -1707,19 +1711,19 @@
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="4">
         <v>2623</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="3">
         <v>80.099999999999994</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="4">
         <v>1276</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="3">
         <v>755.9</v>
       </c>
-      <c r="F56" s="4">
+      <c r="F56" s="3">
         <v>1016.9</v>
       </c>
     </row>
@@ -1727,19 +1731,19 @@
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1747,19 +1751,19 @@
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="4">
         <v>570</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="3">
         <v>62.8</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="4">
         <v>262</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="3">
         <v>507.2</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58" s="3">
         <v>810.6</v>
       </c>
     </row>

</xml_diff>